<commit_message>
update to new extended eligibility format
</commit_message>
<xml_diff>
--- a/libcbm/resources/test/cbm3_tutorial2_eligibilities/sit_input.xlsx
+++ b/libcbm/resources/test/cbm3_tutorial2_eligibilities/sit_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\dev\libcbm\libcbm_py\libcbm\resources\test\cbm3_tutorial2_eligibilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\dev\libcbm\libcbm_py_2.x\libcbm\resources\test\cbm3_tutorial2_eligibilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C91F867-3A05-42DC-94E0-16F7F4746399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05C9B20-95DD-40DB-822B-F0E74C0732E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="10845" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age_classes" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="138">
   <si>
     <t>AGEID20</t>
   </si>
@@ -421,13 +421,31 @@
     <t>disturbance_eligibility_id</t>
   </si>
   <si>
-    <t>pool_filter_expression</t>
-  </si>
-  <si>
-    <t>state_filter_expression</t>
-  </si>
-  <si>
-    <t>(age &gt;= 80) &amp; (age &lt;= 200)</t>
+    <t>expression_type</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>min age</t>
+  </si>
+  <si>
+    <t>max age</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>age &lt;= {p2}</t>
+  </si>
+  <si>
+    <t>age &gt;= {p1}</t>
+  </si>
+  <si>
+    <t>state</t>
   </si>
 </sst>
 </file>
@@ -2226,7 +2244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B45236D-6D2E-48E5-8095-4651482AF9EE}">
   <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -7877,10 +7895,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F32663A-14A4-40CC-942D-649586663DA6}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7888,25 +7906,61 @@
     <col min="1" max="1" width="27.08984375" customWidth="1"/>
     <col min="2" max="2" width="34.90625" customWidth="1"/>
     <col min="3" max="3" width="46.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>128</v>
       </c>
       <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
         <v>129</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update example column naming (disturbance_eligibility_id -> eligibility_id)
</commit_message>
<xml_diff>
--- a/libcbm/resources/test/cbm3_tutorial2_eligibilities/sit_input.xlsx
+++ b/libcbm/resources/test/cbm3_tutorial2_eligibilities/sit_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\dev\libcbm\libcbm_py_2.x\libcbm\resources\test\cbm3_tutorial2_eligibilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\dev\libcbm\libcbm_py_sit_id_extensions\libcbm\resources\test\cbm3_tutorial2_eligibilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05C9B20-95DD-40DB-822B-F0E74C0732E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45326A91-4BEA-42EC-941A-5116C05F4911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5895" yWindow="5385" windowWidth="43200" windowHeight="23445" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age_classes" sheetId="2" r:id="rId1"/>
@@ -418,9 +418,6 @@
     <t>percent</t>
   </si>
   <si>
-    <t>disturbance_eligibility_id</t>
-  </si>
-  <si>
     <t>expression_type</t>
   </si>
   <si>
@@ -446,6 +443,9 @@
   </si>
   <si>
     <t>state</t>
+  </si>
+  <si>
+    <t>eligibility_id</t>
   </si>
 </sst>
 </file>
@@ -769,9 +769,9 @@
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -779,7 +779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -787,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -795,7 +795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -803,7 +803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -811,7 +811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -819,7 +819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -827,7 +827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -835,7 +835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -843,7 +843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -851,7 +851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -859,7 +859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -867,7 +867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -875,7 +875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -883,7 +883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -891,7 +891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -899,7 +899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -907,7 +907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -915,7 +915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -923,7 +923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -931,7 +931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -939,7 +939,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -958,9 +958,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -968,7 +968,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -976,7 +976,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -984,7 +984,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -992,7 +992,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -1011,9 +1011,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1290,9 +1290,9 @@
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -2073,9 +2073,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2244,16 +2244,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B45236D-6D2E-48E5-8095-4651482AF9EE}">
   <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
         <v>76</v>
@@ -2288,7 +2288,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>64</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>64</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>64</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>64</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>64</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>64</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>64</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>64</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>64</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>64</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>64</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>64</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>64</v>
       </c>
@@ -4983,7 +4983,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>64</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>64</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>64</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>64</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>64</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>64</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>64</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>64</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>64</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>64</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>64</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>64</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>64</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>64</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>64</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>64</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>64</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>64</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>64</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>64</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>64</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>64</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>64</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>64</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>64</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>64</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>64</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>64</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>64</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>64</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>64</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>64</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>64</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>64</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>64</v>
       </c>
@@ -6208,7 +6208,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>64</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>64</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>64</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>64</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>64</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>64</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>64</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>64</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>64</v>
       </c>
@@ -6523,7 +6523,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>64</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>64</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>64</v>
       </c>
@@ -6628,7 +6628,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>64</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>64</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>64</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>64</v>
       </c>
@@ -6768,7 +6768,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>64</v>
       </c>
@@ -6803,7 +6803,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>64</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>64</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>64</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>64</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>64</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>64</v>
       </c>
@@ -7013,7 +7013,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>64</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>64</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>64</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>64</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>64</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>64</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>64</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>64</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>64</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>64</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>64</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>64</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>64</v>
       </c>
@@ -7468,7 +7468,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>64</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>64</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>64</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>64</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>64</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>64</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>64</v>
       </c>
@@ -7713,7 +7713,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>64</v>
       </c>
@@ -7748,7 +7748,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>64</v>
       </c>
@@ -7783,7 +7783,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>64</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>64</v>
       </c>
@@ -7853,7 +7853,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>64</v>
       </c>
@@ -7897,67 +7897,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F32663A-14A4-40CC-942D-649586663DA6}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" customWidth="1"/>
-    <col min="2" max="2" width="34.90625" customWidth="1"/>
-    <col min="3" max="3" width="46.81640625" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
         <v>66</v>
       </c>
       <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
         <v>129</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>130</v>
       </c>
-      <c r="E1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>131</v>
-      </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F3">
         <v>200</v>
@@ -7977,9 +7977,9 @@
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -8032,7 +8032,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>

</xml_diff>